<commit_message>
Ran Black and ISORT on codebase
</commit_message>
<xml_diff>
--- a/data/table validation 25 march.xlsx
+++ b/data/table validation 25 march.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\carbonarc\database_tool\build_database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\carbonarc\database_tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9208E7D6-C9E7-4F0A-9B99-9178F90F9272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7482C6F0-E5D4-4632-BB64-BC0ED3E24D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52510" yWindow="750" windowWidth="22620" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32670" yWindow="1050" windowWidth="31200" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table validation" sheetId="1" r:id="rId1"/>
@@ -1458,8 +1458,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="M91" sqref="B90:M91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>